<commit_message>
0.3 - submit to local database
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0701761-C257-49D4-9688-BC146BB1FFB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CC5E55-C431-47C3-BE8B-F22C711E0917}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,27 +417,6 @@
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="8"/>
@@ -468,6 +447,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -482,11 +482,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB1B3937-D9ED-47C1-A2F2-DD049563A215}" name="Πίνακας1" displayName="Πίνακας1" ref="A1:G29" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB1B3937-D9ED-47C1-A2F2-DD049563A215}" name="Πίνακας1" displayName="Πίνακας1" ref="A1:G29" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:G29" xr:uid="{FB1B3937-D9ED-47C1-A2F2-DD049563A215}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9D7D9802-7FB5-4F91-8566-7BB4DB13057F}" name="Όνομα πεδίου"/>
-    <tableColumn id="4" xr3:uid="{F72DF293-DF87-4874-A650-70A6DCBFDAE5}" name="Υποχρεωτική συμπλήρωση" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{F72DF293-DF87-4874-A650-70A6DCBFDAE5}" name="Υποχρεωτική συμπλήρωση" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{11E2B53F-0F3D-4138-AB00-9B5B7D27AB1E}" name="Λατινικό όνομα πεδίου βάσης"/>
     <tableColumn id="2" xr3:uid="{ED07DFBA-70D5-4967-9C0F-67E281749CD0}" name="Τύπος"/>
     <tableColumn id="3" xr3:uid="{7A8A309B-8D26-49D1-904A-3ABDF888068D}" name="Μονάδες μέτρησης"/>
@@ -498,7 +498,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5453EA38-DCA9-4DF1-8E2C-08F4DC58038F}" name="Πίνακας2" displayName="Πίνακας2" ref="A32:G36" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5453EA38-DCA9-4DF1-8E2C-08F4DC58038F}" name="Πίνακας2" displayName="Πίνακας2" ref="A32:G36" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A32:G36" xr:uid="{5453EA38-DCA9-4DF1-8E2C-08F4DC58038F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{37884C31-62D1-4F49-A3C0-D1915ABDDA70}" name="Όνομα πεδίου"/>
@@ -778,7 +778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
0.5 - presented to client
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CC5E55-C431-47C3-BE8B-F22C711E0917}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D3A72A-C585-4891-8DA8-8B3BD644CC1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="93">
   <si>
     <t>Όνομα πεδίου</t>
   </si>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,12 +1236,14 @@
         <v>84</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">

</xml_diff>